<commit_message>
Updated parabricks testing numbers
</commit_message>
<xml_diff>
--- a/Parabricks Testing.xlsx
+++ b/Parabricks Testing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9360" windowHeight="1635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9360" windowHeight="1635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Executive Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="89">
   <si>
     <t>GPU</t>
   </si>
@@ -232,42 +232,6 @@
     <t>[main] CMD: bwa mem -v 3 -Y -K 100000000 -t 9 -R @RG\tID:SUPERFQS01_1_K18088\tLB:K18088\tPU:SUPERFQS01_1\tSM:GIAB_NA12878_1_CL_Whole_C1\tPL:ILLUMINA\tCN:TGen\tPM:HiSeq2500\tBC:ATCACG /home/tgenref/homo_sapiens/grch38_hg38/hg38tgen/tool_resources/bwa_0.7.17/GRCh38tgen_decoy_alts_hla.fa temp/genome/alignment/bwa/GIAB_NA12878_1_CL_Whole_C1_TPFWG/SUPERFQS01_1_K18088/GIAB_NA12878_1_CL_Whole_C1_TPFWG_K18088_SUPERFQS01_NoIndex_L001_R1_001.fastq.gz/02 temp/genome/alignment/bwa/GIAB_NA12878_1_CL_Whole_C1_TPFWG/SUPERFQS01_1_K18088/GIAB_NA12878_1_CL_Whole_C1_TPFWG_K18088_SUPERFQS01_NoIndex_L001_R2_001.fastq.gz/02</t>
   </si>
   <si>
-    <t>[main] Real time: 4757.147 sec; CPU: 41766.798 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 3912.403 sec; CPU: 34133.946 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 3485.429 sec; CPU: 29780.716 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 3915.510 sec; CPU: 34183.683 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 3936.965 sec; CPU: 34364.387 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 4176.779 sec; CPU: 36534.886 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 4918.659 sec; CPU: 43184.085 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 5315.202 sec; CPU: 46370.417 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 3617.139 sec; CPU: 31507.361 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 4052.525 sec; CPU: 35403.717 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 4345.395 sec; CPU: 37338.143 sec</t>
-  </si>
-  <si>
-    <t>[main] Real time: 3397.723 sec; CPU: 29535.457 sec</t>
-  </si>
-  <si>
     <t>[main] Real time: 49830.88 sec; CPU: 434103.6 sec</t>
   </si>
   <si>
@@ -305,6 +269,51 @@
   </si>
   <si>
     <t>5.3 hrs</t>
+  </si>
+  <si>
+    <t>Jetstream Exome pipeline Alignment, Haplotype Caller, Deep Variants</t>
+  </si>
+  <si>
+    <t>USC ORIEN (222M reads)</t>
+  </si>
+  <si>
+    <t>0.7 hrs</t>
+  </si>
+  <si>
+    <t>CPU driven jetstream pipeline for exome data with tgen-style alignment, haplotype caller and deep variants</t>
+  </si>
+  <si>
+    <t>/scratch/gotero/tmp/orien-fastq-batch1</t>
+  </si>
+  <si>
+    <t>[main] CMD: bwa mem -v 3 -Y -K 100000000 -t 9 -R @RG\tID:FLOWCELL_1_SL261775\tLB:SL261775\tPU:FLOWCELL_1\tSM:USCORIEN_A000580_1_KI_Whole_T1\tPL:ILLUMINA\tCN:Hudson Alpha\tPM:.\tBC:unknown /home/tgenref/homo_sapiens/grch38_hg38/hg38tgen/tool_resources/bwa_0.7.17/GRCh38tgen_decoy_alts_hla.fa temp/exome/alignment/bwa/USCORIEN_A000580_1_KI_Whole_T1_KHNE3/FLOWCELL_1_SL261775/SL261775_1.fastq.gz/00 temp/exome/alignment/bwa/USCORIEN_A000580_1_KI_Whole_T1_KHNE3/FLOWCELL_1_SL261775/SL261775_2.fastq.gz/00</t>
+  </si>
+  <si>
+    <t>[main] Real time: 5307.31 sec; CPU: 40914.27 sec</t>
+  </si>
+  <si>
+    <t>46.25 CPUs</t>
+  </si>
+  <si>
+    <t>Deep Variants algorithm</t>
+  </si>
+  <si>
+    <t>GPU driven jetstream pipeline for exome data with parabricks alignment, haplotype caller and deepvairants</t>
+  </si>
+  <si>
+    <t>/scratch/vpagano/pipeline_testing/jetstream_pipelines/CPU-USC-Tight/jetstream/logs</t>
+  </si>
+  <si>
+    <t>/scratch/vpagano/pipeline_testing/jetstream_pipelines/GPU-USC-Tight/jetstream/logs</t>
+  </si>
+  <si>
+    <t>[main] CMD: PARABRICKS mem -Z ./pbOpts.txt -Y -K 100000000 /home/tgenref/homo_sapiens/grch38_hg38/broad_resource_bundle/Homo_sapiens_assembly38.fasta /scratch/vpagano/pipeline_testing/jetstream_pipelines/GPU-USC-Tight/temp/fastqs/SL263838_1.fastq.gz /scratch/vpagano/pipeline_testing/jetstream_pipelines/GPU-USC-Tight/temp/fastqs/SL263838_2.fastq.gz @RG\tID:H7MF3BBXX.8\tLB:lib1\tPL:bar\tSM:sample\tPU:H7MF3BBXX.8</t>
+  </si>
+  <si>
+    <t>[main] Real time: 155.347 sec; CPU: 3058.035 sec</t>
+  </si>
+  <si>
+    <t>19.68 CPUs</t>
   </si>
 </sst>
 </file>
@@ -379,10 +388,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +705,7 @@
         <v>36</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -704,7 +713,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>27154</v>
@@ -715,8 +724,8 @@
       <c r="E2" s="5">
         <v>7.2</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>83</v>
+      <c r="F2" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -735,16 +744,16 @@
       <c r="E3" s="5">
         <v>3.55</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>84</v>
+      <c r="F3" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>24307</v>
@@ -755,8 +764,28 @@
       <c r="E4" s="5">
         <v>4.6900000000000004</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>85</v>
+      <c r="F4" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>3636</v>
+      </c>
+      <c r="D5">
+        <v>1033</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3.52</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -767,16 +796,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N178"/>
+  <dimension ref="A1:B119"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="81.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -785,10 +812,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -895,10 +922,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1005,10 +1032,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -1107,10 +1134,10 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="6"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
@@ -1209,10 +1236,10 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="6"/>
+      <c r="B60" s="7"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
@@ -1283,7 +1310,7 @@
         <v>14</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1291,7 +1318,7 @@
         <v>16</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1319,10 +1346,10 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B75" s="6"/>
+      <c r="B75" s="7"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
@@ -1369,7 +1396,7 @@
         <v>8</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="348" customHeight="1" x14ac:dyDescent="0.25">
@@ -1377,7 +1404,7 @@
         <v>9</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1385,7 +1412,7 @@
         <v>12</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1393,7 +1420,7 @@
         <v>14</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1401,7 +1428,7 @@
         <v>16</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1425,177 +1452,241 @@
         <v>56</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B90" s="7"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" s="4">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="166" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H166" t="s">
-        <v>61</v>
-      </c>
-      <c r="M166">
-        <f>VALUE(MID(H166,SEARCH("Real time:",H166)+11,8))</f>
-        <v>4757.1469999999999</v>
-      </c>
-      <c r="N166">
-        <f>VALUE(MID(H166,SEARCH("CPU:",H166)+5,9))</f>
-        <v>41766.798000000003</v>
-      </c>
-    </row>
-    <row r="167" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H167" t="s">
-        <v>62</v>
-      </c>
-      <c r="M167">
-        <f t="shared" ref="M167:M177" si="0">VALUE(MID(H167,SEARCH("Real time:",H167)+11,8))</f>
-        <v>3912.4029999999998</v>
-      </c>
-      <c r="N167">
-        <f t="shared" ref="N167:N177" si="1">VALUE(MID(H167,SEARCH("CPU:",H167)+5,9))</f>
-        <v>34133.946000000004</v>
-      </c>
-    </row>
-    <row r="168" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H168" t="s">
-        <v>63</v>
-      </c>
-      <c r="M168">
-        <f t="shared" si="0"/>
-        <v>3485.4290000000001</v>
-      </c>
-      <c r="N168">
-        <f t="shared" si="1"/>
-        <v>29780.716</v>
-      </c>
-    </row>
-    <row r="169" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H169" t="s">
-        <v>64</v>
-      </c>
-      <c r="M169">
-        <f t="shared" si="0"/>
-        <v>3915.51</v>
-      </c>
-      <c r="N169">
-        <f t="shared" si="1"/>
-        <v>34183.682999999997</v>
-      </c>
-    </row>
-    <row r="170" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H170" t="s">
-        <v>65</v>
-      </c>
-      <c r="M170">
-        <f t="shared" si="0"/>
-        <v>3936.9650000000001</v>
-      </c>
-      <c r="N170">
-        <f t="shared" si="1"/>
-        <v>34364.387000000002</v>
-      </c>
-    </row>
-    <row r="171" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H171" t="s">
-        <v>66</v>
-      </c>
-      <c r="M171">
-        <f t="shared" si="0"/>
-        <v>4176.7790000000005</v>
-      </c>
-      <c r="N171">
-        <f t="shared" si="1"/>
-        <v>36534.885999999999</v>
-      </c>
-    </row>
-    <row r="172" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H172" t="s">
+    <row r="98" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>16</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>18</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>19</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>82</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B106" s="7"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B107" s="4">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>10</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>7</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>9</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>14</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>18</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>19</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>56</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M172">
-        <f t="shared" si="0"/>
-        <v>4918.6589999999997</v>
-      </c>
-      <c r="N172">
-        <f t="shared" si="1"/>
-        <v>43184.084999999999</v>
-      </c>
-    </row>
-    <row r="173" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H173" t="s">
-        <v>68</v>
-      </c>
-      <c r="M173">
-        <f t="shared" si="0"/>
-        <v>5315.2020000000002</v>
-      </c>
-      <c r="N173">
-        <f t="shared" si="1"/>
-        <v>46370.417000000001</v>
-      </c>
-    </row>
-    <row r="174" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H174" t="s">
-        <v>69</v>
-      </c>
-      <c r="M174">
-        <f t="shared" si="0"/>
-        <v>3617.1390000000001</v>
-      </c>
-      <c r="N174">
-        <f t="shared" si="1"/>
-        <v>31507.361000000001</v>
-      </c>
-    </row>
-    <row r="175" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H175" t="s">
-        <v>70</v>
-      </c>
-      <c r="M175">
-        <f t="shared" si="0"/>
-        <v>4052.5250000000001</v>
-      </c>
-      <c r="N175">
-        <f t="shared" si="1"/>
-        <v>35403.716999999997</v>
-      </c>
-    </row>
-    <row r="176" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H176" t="s">
-        <v>71</v>
-      </c>
-      <c r="M176">
-        <f t="shared" si="0"/>
-        <v>4345.3950000000004</v>
-      </c>
-      <c r="N176">
-        <f t="shared" si="1"/>
-        <v>37338.142999999996</v>
-      </c>
-    </row>
-    <row r="177" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H177" t="s">
-        <v>72</v>
-      </c>
-      <c r="M177">
-        <f t="shared" si="0"/>
-        <v>3397.723</v>
-      </c>
-      <c r="N177">
-        <f t="shared" si="1"/>
-        <v>29535.456999999999</v>
-      </c>
-    </row>
-    <row r="178" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="M178">
-        <f>SUM(M166:M177)</f>
-        <v>49830.876000000004</v>
-      </c>
-      <c r="N178">
-        <f>SUM(N166:N177)</f>
-        <v>434103.59599999996</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A106:B106"/>
     <mergeCell ref="A75:B75"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A17:B17"/>

</xml_diff>